<commit_message>
new way of storing promoted & TL players
</commit_message>
<xml_diff>
--- a/src/data/SkilePromowanychJuniorow1.xlsx
+++ b/src/data/SkilePromowanychJuniorow1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Zawodnik</t>
   </si>
@@ -128,177 +128,21 @@
     <t>Wisz</t>
   </si>
   <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>bd2_s1.png</t>
-  </si>
-  <si>
-    <t>face</t>
-  </si>
-  <si>
-    <t>f2a.png</t>
-  </si>
-  <si>
-    <t>eye</t>
-  </si>
-  <si>
-    <t>e20c.png</t>
-  </si>
-  <si>
-    <t>mouth</t>
-  </si>
-  <si>
-    <t>m32c.png</t>
-  </si>
-  <si>
-    <t>g2.png</t>
-  </si>
-  <si>
-    <t>goatee</t>
-  </si>
-  <si>
-    <t>nose</t>
-  </si>
-  <si>
-    <t>n7.png</t>
-  </si>
-  <si>
-    <t>hair</t>
-  </si>
-  <si>
-    <t>f2h5d.png</t>
-  </si>
-  <si>
-    <t>sympatyczny</t>
-  </si>
-  <si>
-    <t>opanowany</t>
-  </si>
-  <si>
-    <t>uczciwy</t>
-  </si>
-  <si>
     <t>Zbierański</t>
   </si>
   <si>
-    <t>bd3_s1.png</t>
-  </si>
-  <si>
-    <t>f8a.png</t>
-  </si>
-  <si>
-    <t>e24b.png</t>
-  </si>
-  <si>
-    <t>m34b.png</t>
-  </si>
-  <si>
-    <t>n29.png</t>
-  </si>
-  <si>
-    <t>f8h8a.png</t>
-  </si>
-  <si>
     <t>Danik</t>
   </si>
   <si>
-    <t>bd6</t>
-  </si>
-  <si>
-    <t>f4</t>
-  </si>
-  <si>
-    <t>e12c</t>
-  </si>
-  <si>
-    <t>m35c</t>
-  </si>
-  <si>
-    <t>n13</t>
-  </si>
-  <si>
-    <t>h5</t>
-  </si>
-  <si>
-    <t>spokojny</t>
-  </si>
-  <si>
-    <t>podły</t>
-  </si>
-  <si>
-    <t>bd1</t>
-  </si>
-  <si>
-    <t>f6</t>
-  </si>
-  <si>
-    <t>e26c</t>
-  </si>
-  <si>
-    <t>m29c</t>
-  </si>
-  <si>
-    <t>n1</t>
-  </si>
-  <si>
-    <t>h0</t>
-  </si>
-  <si>
     <t>Bochenski</t>
   </si>
   <si>
-    <t>popularny</t>
-  </si>
-  <si>
-    <t>zrownowazony</t>
-  </si>
-  <si>
-    <t>prawy</t>
-  </si>
-  <si>
     <t>Malmur</t>
   </si>
   <si>
-    <t>bd8</t>
-  </si>
-  <si>
-    <t>e36c</t>
-  </si>
-  <si>
-    <t>m3c</t>
-  </si>
-  <si>
-    <t>n19</t>
-  </si>
-  <si>
-    <t>h14</t>
-  </si>
-  <si>
     <t>Szymas</t>
   </si>
   <si>
-    <t>bd7</t>
-  </si>
-  <si>
-    <t>f1</t>
-  </si>
-  <si>
-    <t>e29c</t>
-  </si>
-  <si>
-    <t>m9c</t>
-  </si>
-  <si>
-    <t>przyjemny</t>
-  </si>
-  <si>
-    <t>z charakterem</t>
-  </si>
-  <si>
-    <t>nieuczciwy</t>
-  </si>
-  <si>
     <t>Pakulski</t>
   </si>
   <si>
@@ -342,6 +186,12 @@
   </si>
   <si>
     <t>Maranda</t>
+  </si>
+  <si>
+    <t>Obracaj</t>
+  </si>
+  <si>
+    <t>Swojski</t>
   </si>
 </sst>
 </file>
@@ -681,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z39"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Z1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -698,7 +548,7 @@
     <col min="26" max="26" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -747,29 +597,8 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" t="s">
-        <v>40</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -819,7 +648,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -869,7 +698,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -919,7 +748,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -969,7 +798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1019,7 +848,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1069,7 +898,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1119,7 +948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1169,7 +998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1219,7 +1048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1269,7 +1098,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1319,7 +1148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1369,7 +1198,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1419,7 +1248,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1469,7 +1298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1519,7 +1348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1569,7 +1398,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1619,7 +1448,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1668,40 +1497,17 @@
       <c r="P19">
         <v>4.5</v>
       </c>
-      <c r="Q19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="X19" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26">
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1748,29 +1554,17 @@
       <c r="P20">
         <v>6.5</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-      <c r="V20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26">
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1817,37 +1611,10 @@
       <c r="P21">
         <v>5</v>
       </c>
-      <c r="Q21" t="s">
-        <v>59</v>
-      </c>
-      <c r="R21" t="s">
-        <v>60</v>
-      </c>
-      <c r="S21" t="s">
-        <v>61</v>
-      </c>
-      <c r="T21" t="s">
-        <v>62</v>
-      </c>
-      <c r="V21" t="s">
-        <v>63</v>
-      </c>
-      <c r="W21" t="s">
-        <v>64</v>
-      </c>
-      <c r="X21" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26">
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1894,37 +1661,10 @@
       <c r="P22">
         <v>4.5</v>
       </c>
-      <c r="Q22" t="s">
-        <v>67</v>
-      </c>
-      <c r="R22" t="s">
-        <v>68</v>
-      </c>
-      <c r="S22" t="s">
-        <v>69</v>
-      </c>
-      <c r="T22" t="s">
-        <v>70</v>
-      </c>
-      <c r="V22" t="s">
-        <v>71</v>
-      </c>
-      <c r="W22" t="s">
-        <v>72</v>
-      </c>
-      <c r="X22" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26">
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1971,37 +1711,10 @@
       <c r="P23">
         <v>5.5</v>
       </c>
-      <c r="Q23" t="s">
-        <v>78</v>
-      </c>
-      <c r="R23" t="s">
-        <v>53</v>
-      </c>
-      <c r="S23" t="s">
-        <v>79</v>
-      </c>
-      <c r="T23" t="s">
-        <v>80</v>
-      </c>
-      <c r="V23" t="s">
-        <v>81</v>
-      </c>
-      <c r="W23" t="s">
-        <v>82</v>
-      </c>
-      <c r="X23" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26">
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2048,37 +1761,10 @@
       <c r="P24">
         <v>6.5</v>
       </c>
-      <c r="Q24" t="s">
-        <v>84</v>
-      </c>
-      <c r="R24" t="s">
-        <v>85</v>
-      </c>
-      <c r="S24" t="s">
-        <v>86</v>
-      </c>
-      <c r="T24" t="s">
-        <v>87</v>
-      </c>
-      <c r="V24" t="s">
-        <v>81</v>
-      </c>
-      <c r="W24" t="s">
-        <v>82</v>
-      </c>
-      <c r="X24" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26">
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2126,9 +1812,9 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2177,9 +1863,9 @@
       </c>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2227,9 +1913,9 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2277,9 +1963,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2327,9 +2013,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2377,9 +2063,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:23">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2427,9 +2113,9 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:23">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2479,7 +2165,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2529,7 +2215,7 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2579,7 +2265,7 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2629,7 +2315,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -2679,7 +2365,7 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -2729,7 +2415,7 @@
     </row>
     <row r="38" spans="1:16">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2779,7 +2465,7 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2827,8 +2513,132 @@
         <v>4.5</v>
       </c>
     </row>
+    <row r="40" spans="1:16">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <v>5</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>300</v>
+      </c>
+      <c r="J40">
+        <v>1080</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="L40">
+        <v>4.5</v>
+      </c>
+      <c r="M40">
+        <v>4</v>
+      </c>
+      <c r="N40">
+        <v>4.5</v>
+      </c>
+      <c r="O40">
+        <v>4.5</v>
+      </c>
+      <c r="P40">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>4</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>170</v>
+      </c>
+      <c r="J41">
+        <v>1000</v>
+      </c>
+      <c r="K41">
+        <v>1.5</v>
+      </c>
+      <c r="L41">
+        <v>4</v>
+      </c>
+      <c r="M41">
+        <v>4</v>
+      </c>
+      <c r="N41">
+        <v>2.5</v>
+      </c>
+      <c r="O41">
+        <v>3.5</v>
+      </c>
+      <c r="P41">
+        <v>5.5</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="K5:P5">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6:P6">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7:P7">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -2840,7 +2650,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:P6">
+  <conditionalFormatting sqref="K8:P8">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2852,7 +2662,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7:P7">
+  <conditionalFormatting sqref="K9:P9">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -2864,7 +2674,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:P8">
+  <conditionalFormatting sqref="K10:P10">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -2876,7 +2686,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9:P9">
+  <conditionalFormatting sqref="K12:P12">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -2888,7 +2698,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K10:P10">
+  <conditionalFormatting sqref="K13:P13">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2900,7 +2710,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12:P12">
+  <conditionalFormatting sqref="K14:P14">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -2912,7 +2722,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13:P13">
+  <conditionalFormatting sqref="K16:P16">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -2924,7 +2734,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K14:P14">
+  <conditionalFormatting sqref="K17:P17">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -2936,7 +2746,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K16:P16">
+  <conditionalFormatting sqref="K18:P18">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -2948,7 +2758,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17:P17">
+  <conditionalFormatting sqref="K19:P19">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2960,7 +2770,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18:P18">
+  <conditionalFormatting sqref="K20:P20">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2972,7 +2782,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K19:P19">
+  <conditionalFormatting sqref="K21:P21">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2984,7 +2794,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20:P20">
+  <conditionalFormatting sqref="K22:P22">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -2996,7 +2806,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K21:P21">
+  <conditionalFormatting sqref="K23:P23">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3008,7 +2818,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22:P22">
+  <conditionalFormatting sqref="K26:P26">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3020,7 +2830,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K23:P23">
+  <conditionalFormatting sqref="K27:P27">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3032,7 +2842,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26:P26">
+  <conditionalFormatting sqref="K29:P29">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3044,7 +2854,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27:P27">
+  <conditionalFormatting sqref="K30:P30">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3056,7 +2866,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29:P29">
+  <conditionalFormatting sqref="K31:P31">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3068,7 +2878,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30:P30">
+  <conditionalFormatting sqref="K37:P37">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3080,7 +2890,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K31:P31">
+  <conditionalFormatting sqref="K39:P39">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3092,7 +2902,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K37:P37">
+  <conditionalFormatting sqref="K40:P40">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3104,7 +2914,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K39:P39">
+  <conditionalFormatting sqref="K41:P41">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3116,22 +2926,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="Q19" r:id="rId1" display="https://www82.hattrick.org/Img/Avatar/bodies/bd2_s1.png"/>
-    <hyperlink ref="R19" r:id="rId2" display="https://www82.hattrick.org/Img/Avatar/faces/f2a.png"/>
-    <hyperlink ref="S19" r:id="rId3" display="https://www82.hattrick.org/Img/Avatar/eyes/e20c.png"/>
-    <hyperlink ref="T19" r:id="rId4" display="https://www82.hattrick.org/Img/Avatar/mouths/m32c.png"/>
-    <hyperlink ref="U19" r:id="rId5" display="https://www82.hattrick.org/Img/Avatar/goatees/g2.png"/>
-    <hyperlink ref="V19" r:id="rId6" display="https://www82.hattrick.org/Img/Avatar/noses/n7.png"/>
-    <hyperlink ref="W19" r:id="rId7" display="https://www82.hattrick.org/Img/Avatar/hair/f2h5d.png"/>
-    <hyperlink ref="Q20" r:id="rId8" display="https://www89.hattrick.org/Img/Avatar/bodies/bd3_s1.png"/>
-    <hyperlink ref="R20" r:id="rId9" display="https://www89.hattrick.org/Img/Avatar/faces/f8a.png"/>
-    <hyperlink ref="S20" r:id="rId10" display="https://www89.hattrick.org/Img/Avatar/eyes/e24b.png"/>
-    <hyperlink ref="T20" r:id="rId11" display="https://www89.hattrick.org/Img/Avatar/mouths/m34b.png"/>
-    <hyperlink ref="V20" r:id="rId12" display="https://www89.hattrick.org/Img/Avatar/noses/n29.png"/>
-    <hyperlink ref="W20" r:id="rId13" display="https://www89.hattrick.org/Img/Avatar/hair/f8h8a.png"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
db update + small work on creating U21 schedule
</commit_message>
<xml_diff>
--- a/src/data/SkilePromowanychJuniorow1.xlsx
+++ b/src/data/SkilePromowanychJuniorow1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Zawodnik</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>Patyk</t>
+  </si>
+  <si>
+    <t>Herma</t>
   </si>
 </sst>
 </file>
@@ -573,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W55"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L59" sqref="L59"/>
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3355,8 +3358,70 @@
         <v>4</v>
       </c>
     </row>
+    <row r="56" spans="1:16">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>5</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56">
+        <v>410</v>
+      </c>
+      <c r="J56">
+        <v>1160</v>
+      </c>
+      <c r="K56">
+        <v>2.5</v>
+      </c>
+      <c r="L56">
+        <v>5</v>
+      </c>
+      <c r="M56">
+        <v>5</v>
+      </c>
+      <c r="N56">
+        <v>4</v>
+      </c>
+      <c r="O56">
+        <v>4</v>
+      </c>
+      <c r="P56">
+        <v>5.5</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="K5:P5">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6:P6">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -3368,7 +3433,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:P6">
+  <conditionalFormatting sqref="K7:P7">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -3380,7 +3445,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7:P7">
+  <conditionalFormatting sqref="K8:P8">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -3392,7 +3457,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:P8">
+  <conditionalFormatting sqref="K9:P9">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -3404,7 +3469,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9:P9">
+  <conditionalFormatting sqref="K10:P10">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -3416,7 +3481,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K10:P10">
+  <conditionalFormatting sqref="K11:P11">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -3428,7 +3493,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K11:P11">
+  <conditionalFormatting sqref="K12:P12">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -3440,7 +3505,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12:P12">
+  <conditionalFormatting sqref="K13:P13">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -3452,7 +3517,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13:P13">
+  <conditionalFormatting sqref="K15:P15">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -3464,7 +3529,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K15:P15">
+  <conditionalFormatting sqref="K16:P16">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -3476,7 +3541,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K16:P16">
+  <conditionalFormatting sqref="K17:P17">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -3488,7 +3553,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17:P17">
+  <conditionalFormatting sqref="K18:P18">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -3500,7 +3565,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18:P18">
+  <conditionalFormatting sqref="K19:P19">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -3512,7 +3577,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K19:P19">
+  <conditionalFormatting sqref="K20:P20">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -3524,7 +3589,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20:P20">
+  <conditionalFormatting sqref="K21:P21">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -3536,7 +3601,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K21:P21">
+  <conditionalFormatting sqref="K22:P22">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -3548,7 +3613,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22:P22">
+  <conditionalFormatting sqref="K25:P25">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -3560,7 +3625,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K25:P25">
+  <conditionalFormatting sqref="K26:P26">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -3572,7 +3637,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26:P26">
+  <conditionalFormatting sqref="K28:P28">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -3584,7 +3649,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28:P28">
+  <conditionalFormatting sqref="K29:P29">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -3596,7 +3661,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29:P29">
+  <conditionalFormatting sqref="K30:P30">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -3608,7 +3673,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30:P30">
+  <conditionalFormatting sqref="K36:P36">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -3620,7 +3685,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K36:P36">
+  <conditionalFormatting sqref="K38:P38">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -3632,7 +3697,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K38:P38">
+  <conditionalFormatting sqref="K39:P39">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -3644,7 +3709,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K39:P39">
+  <conditionalFormatting sqref="K40:P40">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -3656,7 +3721,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K40:P40">
+  <conditionalFormatting sqref="K41:P41">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -3668,7 +3733,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:P41">
+  <conditionalFormatting sqref="K42:P42">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3680,19 +3745,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K42:P42">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K44:P44">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K45:P45">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -3704,7 +3769,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K45:P45">
+  <conditionalFormatting sqref="K46:P46">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3716,19 +3781,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46:P46">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K47:P47">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48:P48">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3740,7 +3805,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K48:P48">
+  <conditionalFormatting sqref="K49:P49">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -3752,7 +3817,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K49:P49">
+  <conditionalFormatting sqref="K50:P50">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -3764,7 +3829,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K50:P50">
+  <conditionalFormatting sqref="K51:P51">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -3776,7 +3841,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K51:P51">
+  <conditionalFormatting sqref="K52:P52">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3788,7 +3853,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K52:P52">
+  <conditionalFormatting sqref="K53:P53">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3800,7 +3865,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K53:P53">
+  <conditionalFormatting sqref="K2:P43">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:H56 I56:J56">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3811,20 +3888,28 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:P43">
-    <cfRule type="colorScale" priority="49">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H55">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:P53">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3835,64 +3920,44 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K54:P54">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:P54">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
+        <color theme="0"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K55:P55">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color theme="0"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:P53">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K54:P54">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:P54">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K55:P55">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56:P56">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>